<commit_message>
:memo: Add & Update exam, result
</commit_message>
<xml_diff>
--- a/Exam/ExamQuestion.xlsx
+++ b/Exam/ExamQuestion.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ponmorin/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyProject\Contextual-Retrieval\Exam\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A93E353-2457-9F45-83B6-A6955E853E97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53AC13FE-3092-48E8-A32C-B6A6B610F30B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16260" xr2:uid="{8D1546C2-F62A-314F-87B7-76B574C6FD06}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8D1546C2-F62A-314F-87B7-76B574C6FD06}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -335,9 +335,6 @@
     <t>instruction</t>
   </si>
   <si>
-    <t>result</t>
-  </si>
-  <si>
     <t>วิศวกรรมศาสตรบัณฑิต (วิศวกรรมคอมพิวเตอร์)</t>
   </si>
   <si>
@@ -627,6 +624,9 @@
   </si>
   <si>
     <t>45 หน่วยกิต</t>
+  </si>
+  <si>
+    <t>ref_answer</t>
   </si>
 </sst>
 </file>
@@ -692,7 +692,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -706,9 +706,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -735,9 +732,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -775,7 +772,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -881,7 +878,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1023,7 +1020,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1034,17 +1031,17 @@
   <dimension ref="A1:C101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.33203125" customWidth="1"/>
-    <col min="2" max="2" width="96.83203125" customWidth="1"/>
+    <col min="1" max="1" width="7.375" customWidth="1"/>
+    <col min="2" max="2" width="96.875" customWidth="1"/>
     <col min="3" max="3" width="50" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>97</v>
       </c>
@@ -1052,10 +1049,10 @@
         <v>98</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="22" x14ac:dyDescent="0.25">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1063,32 +1060,32 @@
         <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="22" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="22" x14ac:dyDescent="0.25">
+      <c r="C3" s="7" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="22" x14ac:dyDescent="0.25">
+      <c r="C4" s="7" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1096,10 +1093,10 @@
         <v>3</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="22" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1107,21 +1104,21 @@
         <v>92</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="22" x14ac:dyDescent="0.25">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="9" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="44" x14ac:dyDescent="0.25">
+      <c r="C7" s="8" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="42" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1129,10 +1126,10 @@
         <v>5</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="22" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1140,10 +1137,10 @@
         <v>6</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="22" x14ac:dyDescent="0.25">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -1151,10 +1148,10 @@
         <v>7</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="44" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -1162,10 +1159,10 @@
         <v>8</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="22" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -1173,10 +1170,10 @@
         <v>9</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="22" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -1184,10 +1181,10 @@
         <v>10</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="22" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -1195,10 +1192,10 @@
         <v>11</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="22" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -1206,10 +1203,10 @@
         <v>12</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="22" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -1217,10 +1214,10 @@
         <v>13</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="44" x14ac:dyDescent="0.25">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="42" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -1228,10 +1225,10 @@
         <v>14</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="44" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -1239,10 +1236,10 @@
         <v>93</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="44" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="42" x14ac:dyDescent="0.35">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -1250,10 +1247,10 @@
         <v>15</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="44" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="42" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -1261,10 +1258,10 @@
         <v>16</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="66" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="42" x14ac:dyDescent="0.35">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -1272,10 +1269,10 @@
         <v>17</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="44" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -1283,21 +1280,21 @@
         <v>18</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="22" x14ac:dyDescent="0.2">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>22</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C23" s="9" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="22" x14ac:dyDescent="0.25">
+      <c r="C23" s="8" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -1305,10 +1302,10 @@
         <v>20</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="44" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="42" x14ac:dyDescent="0.35">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -1316,10 +1313,10 @@
         <v>21</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="22" x14ac:dyDescent="0.25">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -1327,10 +1324,10 @@
         <v>94</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="22" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -1338,10 +1335,10 @@
         <v>22</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="22" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -1349,10 +1346,10 @@
         <v>23</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="22" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -1360,10 +1357,10 @@
         <v>24</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="44" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -1371,10 +1368,10 @@
         <v>25</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="44" x14ac:dyDescent="0.25">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="42" x14ac:dyDescent="0.35">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -1382,10 +1379,10 @@
         <v>26</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="22" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -1393,10 +1390,10 @@
         <v>27</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="22" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -1404,10 +1401,10 @@
         <v>28</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="22" x14ac:dyDescent="0.25">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -1415,10 +1412,10 @@
         <v>29</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="22" x14ac:dyDescent="0.25">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -1426,10 +1423,10 @@
         <v>30</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="22" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A36" s="2">
         <v>35</v>
       </c>
@@ -1437,10 +1434,10 @@
         <v>95</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="44" x14ac:dyDescent="0.25">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="42" x14ac:dyDescent="0.35">
       <c r="A37" s="2">
         <v>36</v>
       </c>
@@ -1448,10 +1445,10 @@
         <v>96</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="44" x14ac:dyDescent="0.25">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A38" s="2">
         <v>37</v>
       </c>
@@ -1459,10 +1456,10 @@
         <v>31</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="22" x14ac:dyDescent="0.25">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A39" s="2">
         <v>38</v>
       </c>
@@ -1470,10 +1467,10 @@
         <v>32</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="44" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A40" s="2">
         <v>39</v>
       </c>
@@ -1481,10 +1478,10 @@
         <v>33</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="44" x14ac:dyDescent="0.25">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A41" s="2">
         <v>40</v>
       </c>
@@ -1492,10 +1489,10 @@
         <v>34</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="22" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A42" s="2">
         <v>41</v>
       </c>
@@ -1503,10 +1500,10 @@
         <v>35</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="22" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A43" s="2">
         <v>42</v>
       </c>
@@ -1514,10 +1511,10 @@
         <v>36</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" ht="22" x14ac:dyDescent="0.25">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A44" s="2">
         <v>43</v>
       </c>
@@ -1525,10 +1522,10 @@
         <v>37</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" ht="22" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A45" s="2">
         <v>44</v>
       </c>
@@ -1536,10 +1533,10 @@
         <v>38</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" ht="22" x14ac:dyDescent="0.25">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A46" s="2">
         <v>45</v>
       </c>
@@ -1547,10 +1544,10 @@
         <v>39</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" ht="22" x14ac:dyDescent="0.25">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A47" s="2">
         <v>46</v>
       </c>
@@ -1558,10 +1555,10 @@
         <v>2</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" ht="22" x14ac:dyDescent="0.25">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A48" s="2">
         <v>47</v>
       </c>
@@ -1569,10 +1566,10 @@
         <v>40</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" ht="22" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A49" s="2">
         <v>48</v>
       </c>
@@ -1580,10 +1577,10 @@
         <v>41</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" ht="22" x14ac:dyDescent="0.25">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A50" s="2">
         <v>49</v>
       </c>
@@ -1591,10 +1588,10 @@
         <v>42</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" ht="22" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A51" s="2">
         <v>50</v>
       </c>
@@ -1602,21 +1599,21 @@
         <v>43</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" ht="22" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A52" s="2">
         <v>51</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C52" s="8" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" ht="44" x14ac:dyDescent="0.25">
+      <c r="C52" s="7" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A53" s="2">
         <v>52</v>
       </c>
@@ -1624,10 +1621,10 @@
         <v>45</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" ht="22" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A54" s="2">
         <v>53</v>
       </c>
@@ -1635,10 +1632,10 @@
         <v>46</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" ht="22" x14ac:dyDescent="0.25">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A55" s="2">
         <v>54</v>
       </c>
@@ -1646,10 +1643,10 @@
         <v>47</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" ht="22" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A56" s="2">
         <v>55</v>
       </c>
@@ -1657,10 +1654,10 @@
         <v>48</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" ht="22" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A57" s="2">
         <v>56</v>
       </c>
@@ -1668,10 +1665,10 @@
         <v>49</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" ht="22" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A58" s="2">
         <v>57</v>
       </c>
@@ -1679,10 +1676,10 @@
         <v>50</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" ht="22" x14ac:dyDescent="0.25">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A59" s="2">
         <v>58</v>
       </c>
@@ -1690,21 +1687,21 @@
         <v>51</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" ht="22" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A60" s="2">
         <v>59</v>
       </c>
       <c r="B60" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C60" s="8" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" ht="22" x14ac:dyDescent="0.25">
+      <c r="C60" s="7" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A61" s="2">
         <v>60</v>
       </c>
@@ -1712,10 +1709,10 @@
         <v>53</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" ht="22" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A62" s="2">
         <v>61</v>
       </c>
@@ -1723,10 +1720,10 @@
         <v>54</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" ht="22" x14ac:dyDescent="0.25">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A63" s="2">
         <v>62</v>
       </c>
@@ -1734,10 +1731,10 @@
         <v>55</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" ht="22" x14ac:dyDescent="0.25">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A64" s="2">
         <v>63</v>
       </c>
@@ -1745,10 +1742,10 @@
         <v>56</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" ht="22" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A65" s="2">
         <v>64</v>
       </c>
@@ -1756,10 +1753,10 @@
         <v>57</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" ht="22" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A66" s="2">
         <v>65</v>
       </c>
@@ -1767,10 +1764,10 @@
         <v>58</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" ht="22" x14ac:dyDescent="0.25">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A67" s="2">
         <v>66</v>
       </c>
@@ -1778,10 +1775,10 @@
         <v>59</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" ht="22" x14ac:dyDescent="0.25">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A68" s="2">
         <v>67</v>
       </c>
@@ -1789,10 +1786,10 @@
         <v>60</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" ht="22" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A69" s="2">
         <v>68</v>
       </c>
@@ -1800,10 +1797,10 @@
         <v>61</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" ht="44" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A70" s="2">
         <v>69</v>
       </c>
@@ -1811,10 +1808,10 @@
         <v>62</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" ht="22" x14ac:dyDescent="0.25">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A71" s="2">
         <v>70</v>
       </c>
@@ -1822,10 +1819,10 @@
         <v>63</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" ht="44" x14ac:dyDescent="0.25">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A72" s="2">
         <v>71</v>
       </c>
@@ -1833,21 +1830,21 @@
         <v>64</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" ht="44" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A73" s="2">
         <v>72</v>
       </c>
       <c r="B73" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C73" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="C73" s="3" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" ht="44" x14ac:dyDescent="0.25">
+    </row>
+    <row r="74" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A74" s="2">
         <v>73</v>
       </c>
@@ -1855,10 +1852,10 @@
         <v>65</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" ht="22" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A75" s="2">
         <v>74</v>
       </c>
@@ -1866,10 +1863,10 @@
         <v>66</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" ht="44" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A76" s="2">
         <v>75</v>
       </c>
@@ -1877,10 +1874,10 @@
         <v>67</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" ht="22" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A77" s="2">
         <v>76</v>
       </c>
@@ -1888,10 +1885,10 @@
         <v>68</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" ht="22" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A78" s="2">
         <v>77</v>
       </c>
@@ -1899,10 +1896,10 @@
         <v>69</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" ht="22" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A79" s="2">
         <v>78</v>
       </c>
@@ -1910,10 +1907,10 @@
         <v>70</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" ht="22" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A80" s="2">
         <v>79</v>
       </c>
@@ -1921,10 +1918,10 @@
         <v>71</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" ht="22" x14ac:dyDescent="0.25">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A81" s="2">
         <v>80</v>
       </c>
@@ -1932,10 +1929,10 @@
         <v>72</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" ht="22" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A82" s="2">
         <v>81</v>
       </c>
@@ -1943,10 +1940,10 @@
         <v>73</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" ht="22" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A83" s="2">
         <v>82</v>
       </c>
@@ -1954,21 +1951,21 @@
         <v>74</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" ht="22" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A84" s="2">
         <v>83</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" ht="88" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" ht="63" x14ac:dyDescent="0.35">
       <c r="A85" s="2">
         <v>84</v>
       </c>
@@ -1976,21 +1973,21 @@
         <v>75</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" ht="44" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" ht="42" x14ac:dyDescent="0.35">
       <c r="A86" s="2">
         <v>85</v>
       </c>
       <c r="B86" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="C86" s="7" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" ht="88" x14ac:dyDescent="0.25">
+      <c r="C86" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" ht="63" x14ac:dyDescent="0.35">
       <c r="A87" s="2">
         <v>86</v>
       </c>
@@ -1998,10 +1995,10 @@
         <v>77</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" ht="22" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A88" s="2">
         <v>87</v>
       </c>
@@ -2009,10 +2006,10 @@
         <v>78</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" ht="22" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A89" s="2">
         <v>88</v>
       </c>
@@ -2020,10 +2017,10 @@
         <v>79</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" ht="22" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A90" s="2">
         <v>89</v>
       </c>
@@ -2031,10 +2028,10 @@
         <v>80</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" ht="44" x14ac:dyDescent="0.25">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A91" s="2">
         <v>90</v>
       </c>
@@ -2042,10 +2039,10 @@
         <v>81</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" ht="44" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A92" s="2">
         <v>91</v>
       </c>
@@ -2053,10 +2050,10 @@
         <v>82</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" ht="22" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A93" s="2">
         <v>92</v>
       </c>
@@ -2064,10 +2061,10 @@
         <v>83</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" ht="22" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A94" s="2">
         <v>93</v>
       </c>
@@ -2075,10 +2072,10 @@
         <v>84</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" ht="44" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A95" s="2">
         <v>94</v>
       </c>
@@ -2086,10 +2083,10 @@
         <v>85</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" ht="44" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A96" s="2">
         <v>95</v>
       </c>
@@ -2097,10 +2094,10 @@
         <v>86</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" ht="22" x14ac:dyDescent="0.25">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A97" s="2">
         <v>96</v>
       </c>
@@ -2108,10 +2105,10 @@
         <v>87</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" ht="22" x14ac:dyDescent="0.25">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A98" s="2">
         <v>97</v>
       </c>
@@ -2119,10 +2116,10 @@
         <v>88</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" ht="44" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A99" s="2">
         <v>98</v>
       </c>
@@ -2130,10 +2127,10 @@
         <v>89</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" ht="22" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A100" s="2">
         <v>99</v>
       </c>
@@ -2141,10 +2138,10 @@
         <v>90</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" ht="22" x14ac:dyDescent="0.25">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A101" s="2">
         <v>100</v>
       </c>
@@ -2152,7 +2149,7 @@
         <v>91</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>